<commit_message>
Added Resource for ExportServices
</commit_message>
<xml_diff>
--- a/Tasks.xlsx
+++ b/Tasks.xlsx
@@ -476,7 +476,7 @@
   <dimension ref="A1:C20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -667,7 +667,10 @@
         <v>20</v>
       </c>
       <c r="B18" t="s">
-        <v>21</v>
+        <v>5</v>
+      </c>
+      <c r="C18" s="7">
+        <v>42893</v>
       </c>
     </row>
     <row r="19" spans="1:3">

</xml_diff>

<commit_message>
- Updated .net Framework - Added ViewModels - Excel & PDF Bugs Fixes -
</commit_message>
<xml_diff>
--- a/Tasks.xlsx
+++ b/Tasks.xlsx
@@ -1,21 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20385" windowHeight="8355"/>
+    <workbookView windowWidth="20385" windowHeight="8370"/>
   </bookViews>
   <sheets>
     <sheet name="Tasks" sheetId="1" r:id="rId1"/>
-    <sheet name="References" sheetId="2" r:id="rId2"/>
+    <sheet name="Bug Fixes" sheetId="2" r:id="rId2"/>
+    <sheet name="PBI's" sheetId="3" r:id="rId3"/>
+    <sheet name="References" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="144525" iterate="1" iterateCount="100" iterateDelta="0.001"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46">
   <si>
     <t>Haenggi Model Calculator</t>
   </si>
@@ -29,12 +31,15 @@
     <t>Last Update</t>
   </si>
   <si>
+    <t>Add Model Project</t>
+  </si>
+  <si>
+    <t>Done</t>
+  </si>
+  <si>
     <t xml:space="preserve">Exportar resultados a PDF </t>
   </si>
   <si>
-    <t>Done</t>
-  </si>
-  <si>
     <t>Cambio de textbox al tomar muestra</t>
   </si>
   <si>
@@ -71,15 +76,78 @@
     <t xml:space="preserve">Implement MVVM </t>
   </si>
   <si>
+    <t>Importacion de Excel a Programa</t>
+  </si>
+  <si>
     <t>Pending</t>
   </si>
   <si>
-    <t>Importacion de Excel a Programa</t>
-  </si>
-  <si>
     <t>Add a Common Resource Project</t>
   </si>
   <si>
+    <t>Move to Framework 4.6.1</t>
+  </si>
+  <si>
+    <t>Add validation to only support Numbers</t>
+  </si>
+  <si>
+    <t>Implement MVVM  Command</t>
+  </si>
+  <si>
+    <t>Move to .NET Core</t>
+  </si>
+  <si>
+    <t>Setup Install custom</t>
+  </si>
+  <si>
+    <t>Modulo</t>
+  </si>
+  <si>
+    <t>Sub Modulo</t>
+  </si>
+  <si>
+    <t>Descripcion</t>
+  </si>
+  <si>
+    <t>Estado</t>
+  </si>
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>Excel</t>
+  </si>
+  <si>
+    <t>Hoja medidas</t>
+  </si>
+  <si>
+    <t>Date is not assigned</t>
+  </si>
+  <si>
+    <t>Sacar boton Ayuda</t>
+  </si>
+  <si>
+    <t>Sacar boton Comentarios</t>
+  </si>
+  <si>
+    <t>Sacar Firma y Especialista</t>
+  </si>
+  <si>
+    <t>Hoja Resultados</t>
+  </si>
+  <si>
+    <t>Sacar imagen de pinza</t>
+  </si>
+  <si>
+    <t>PDF</t>
+  </si>
+  <si>
+    <t>Titulos</t>
+  </si>
+  <si>
+    <t>Revisar titulos</t>
+  </si>
+  <si>
     <t>In Progress</t>
   </si>
   <si>
@@ -87,25 +155,20 @@
   </si>
   <si>
     <t>Blocked</t>
-  </si>
-  <si>
-    <t>Add Model Project</t>
-  </si>
-  <si>
-    <t>Move to Framework 4.6.1</t>
-  </si>
-  <si>
-    <t>Add validation to only support Numbers</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="dd/mm/yyyy;@"/>
+  <numFmts count="5">
+    <numFmt numFmtId="176" formatCode="dd/mm/yyyy;@"/>
+    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
-  <fonts count="2">
+  <fonts count="21">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -117,10 +180,155 @@
       <sz val="11"/>
       <color theme="0"/>
       <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="33">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -129,18 +337,192 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4"/>
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -148,56 +530,335 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="9" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="8" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="22" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="12" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="5" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="31"/>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="34" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="31" applyAlignment="1"/>
+    <xf numFmtId="176" fontId="1" fillId="2" borderId="0" xfId="31" applyNumberFormat="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="58" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="1" applyAlignment="1"/>
-    <xf numFmtId="164" fontId="1" fillId="3" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="2" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
+    <xf numFmtId="58" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="3">
-    <cellStyle name="Énfasis1" xfId="1" builtinId="29"/>
-    <cellStyle name="Énfasis2" xfId="2" builtinId="33"/>
+  <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="40% - Accent1" xfId="1" builtinId="31"/>
+    <cellStyle name="Comma" xfId="2" builtinId="3"/>
+    <cellStyle name="Comma [0]" xfId="3" builtinId="6"/>
+    <cellStyle name="Currency [0]" xfId="4" builtinId="7"/>
+    <cellStyle name="Currency" xfId="5" builtinId="4"/>
+    <cellStyle name="Percent" xfId="6" builtinId="5"/>
+    <cellStyle name="Check Cell" xfId="7" builtinId="23"/>
+    <cellStyle name="Heading 2" xfId="8" builtinId="17"/>
+    <cellStyle name="Note" xfId="9" builtinId="10"/>
+    <cellStyle name="Hyperlink" xfId="10" builtinId="8"/>
+    <cellStyle name="60% - Accent4" xfId="11" builtinId="44"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9"/>
+    <cellStyle name="40% - Accent3" xfId="13" builtinId="39"/>
+    <cellStyle name="Warning Text" xfId="14" builtinId="11"/>
+    <cellStyle name="40% - Accent2" xfId="15" builtinId="35"/>
+    <cellStyle name="Title" xfId="16" builtinId="15"/>
+    <cellStyle name="CExplanatory Text" xfId="17" builtinId="53"/>
+    <cellStyle name="Heading 1" xfId="18" builtinId="16"/>
+    <cellStyle name="Heading 3" xfId="19" builtinId="18"/>
+    <cellStyle name="Heading 4" xfId="20" builtinId="19"/>
+    <cellStyle name="Input" xfId="21" builtinId="20"/>
+    <cellStyle name="60% - Accent3" xfId="22" builtinId="40"/>
+    <cellStyle name="Good" xfId="23" builtinId="26"/>
+    <cellStyle name="Output" xfId="24" builtinId="21"/>
+    <cellStyle name="20% - Accent1" xfId="25" builtinId="30"/>
+    <cellStyle name="Calculation" xfId="26" builtinId="22"/>
+    <cellStyle name="Linked Cell" xfId="27" builtinId="24"/>
+    <cellStyle name="Total" xfId="28" builtinId="25"/>
+    <cellStyle name="Bad" xfId="29" builtinId="27"/>
+    <cellStyle name="Neutral" xfId="30" builtinId="28"/>
+    <cellStyle name="Accent1" xfId="31" builtinId="29"/>
+    <cellStyle name="20% - Accent5" xfId="32" builtinId="46"/>
+    <cellStyle name="60% - Accent1" xfId="33" builtinId="32"/>
+    <cellStyle name="Accent2" xfId="34" builtinId="33"/>
+    <cellStyle name="20% - Accent2" xfId="35" builtinId="34"/>
+    <cellStyle name="20% - Accent6" xfId="36" builtinId="50"/>
+    <cellStyle name="60% - Accent2" xfId="37" builtinId="36"/>
+    <cellStyle name="Accent3" xfId="38" builtinId="37"/>
+    <cellStyle name="20% - Accent3" xfId="39" builtinId="38"/>
+    <cellStyle name="Accent4" xfId="40" builtinId="41"/>
+    <cellStyle name="20% - Accent4" xfId="41" builtinId="42"/>
+    <cellStyle name="40% - Accent4" xfId="42" builtinId="43"/>
+    <cellStyle name="Accent5" xfId="43" builtinId="45"/>
+    <cellStyle name="40% - Accent5" xfId="44" builtinId="47"/>
+    <cellStyle name="60% - Accent5" xfId="45" builtinId="48"/>
+    <cellStyle name="Accent6" xfId="46" builtinId="49"/>
+    <cellStyle name="40% - Accent6" xfId="47" builtinId="51"/>
+    <cellStyle name="60% - Accent6" xfId="48" builtinId="52"/>
   </cellStyles>
-  <dxfs count="1">
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
-    </dxf>
-  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2"/>
 </styleSheet>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabla1" displayName="Tabla1" ref="A2:C20" totalsRowShown="0">
-  <autoFilter ref="A2:C20"/>
-  <sortState ref="A3:C18">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabla1" displayName="Tabla1" ref="A2:C23" totalsRowShown="0">
+  <autoFilter ref="A2:C23"/>
+  <sortState ref="A2:C23">
     <sortCondition ref="B3:B18"/>
     <sortCondition ref="C3:C18"/>
   </sortState>
   <tableColumns count="3">
-    <tableColumn id="1" name="Item" dataDxfId="0"/>
+    <tableColumn id="1" name="Item"/>
     <tableColumn id="2" name="Status"/>
     <tableColumn id="3" name="Last Update"/>
   </tableColumns>
@@ -206,6 +867,19 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table4" displayName="Table4" ref="A2:E10" headerRowCount="0" totalsRowShown="0">
+  <tableColumns count="5">
+    <tableColumn id="1" name="Column1"/>
+    <tableColumn id="2" name="Column5"/>
+    <tableColumn id="3" name="Column2"/>
+    <tableColumn id="4" name="Column3"/>
+    <tableColumn id="5" name="Column4"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium23" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="A1:A6" totalsRowShown="0">
   <autoFilter ref="A1:A6"/>
   <tableColumns count="1">
@@ -467,56 +1141,57 @@
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
-  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C20"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr/>
+  <dimension ref="A1:C23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelCol="2"/>
   <cols>
-    <col min="1" max="1" width="57.42578125" customWidth="1"/>
-    <col min="3" max="3" width="13.42578125" customWidth="1"/>
+    <col min="1" max="1" width="57.4285714285714" customWidth="1"/>
+    <col min="2" max="2" width="11.4285714285714" customWidth="1"/>
+    <col min="3" max="3" width="13.4285714285714" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="8"/>
-      <c r="C1" s="8"/>
+      <c r="B1" s="3"/>
+      <c r="C1" s="3"/>
     </row>
     <row r="2" spans="1:3">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="5" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:3">
-      <c r="A3" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="B3" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="C3" s="7">
+      <c r="A3" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="8">
         <v>42862</v>
       </c>
     </row>
     <row r="4" spans="1:3">
-      <c r="A4" s="1" t="s">
-        <v>4</v>
+      <c r="A4" s="9" t="s">
+        <v>6</v>
       </c>
       <c r="B4" t="s">
         <v>5</v>
@@ -526,8 +1201,8 @@
       </c>
     </row>
     <row r="5" spans="1:3">
-      <c r="A5" s="1" t="s">
-        <v>6</v>
+      <c r="A5" s="9" t="s">
+        <v>7</v>
       </c>
       <c r="B5" t="s">
         <v>5</v>
@@ -537,8 +1212,8 @@
       </c>
     </row>
     <row r="6" spans="1:3">
-      <c r="A6" s="1" t="s">
-        <v>7</v>
+      <c r="A6" s="9" t="s">
+        <v>8</v>
       </c>
       <c r="B6" t="s">
         <v>5</v>
@@ -548,8 +1223,8 @@
       </c>
     </row>
     <row r="7" spans="1:3">
-      <c r="A7" s="1" t="s">
-        <v>8</v>
+      <c r="A7" s="9" t="s">
+        <v>9</v>
       </c>
       <c r="B7" t="s">
         <v>5</v>
@@ -559,8 +1234,8 @@
       </c>
     </row>
     <row r="8" spans="1:3">
-      <c r="A8" s="1" t="s">
-        <v>9</v>
+      <c r="A8" s="9" t="s">
+        <v>10</v>
       </c>
       <c r="B8" t="s">
         <v>5</v>
@@ -570,8 +1245,8 @@
       </c>
     </row>
     <row r="9" spans="1:3">
-      <c r="A9" s="1" t="s">
-        <v>10</v>
+      <c r="A9" s="9" t="s">
+        <v>11</v>
       </c>
       <c r="B9" t="s">
         <v>5</v>
@@ -581,8 +1256,8 @@
       </c>
     </row>
     <row r="10" spans="1:3">
-      <c r="A10" s="1" t="s">
-        <v>11</v>
+      <c r="A10" s="9" t="s">
+        <v>12</v>
       </c>
       <c r="B10" t="s">
         <v>5</v>
@@ -592,8 +1267,8 @@
       </c>
     </row>
     <row r="11" spans="1:3">
-      <c r="A11" s="1" t="s">
-        <v>12</v>
+      <c r="A11" s="9" t="s">
+        <v>13</v>
       </c>
       <c r="B11" t="s">
         <v>5</v>
@@ -603,8 +1278,8 @@
       </c>
     </row>
     <row r="12" spans="1:3">
-      <c r="A12" s="1" t="s">
-        <v>13</v>
+      <c r="A12" s="9" t="s">
+        <v>14</v>
       </c>
       <c r="B12" t="s">
         <v>5</v>
@@ -614,8 +1289,8 @@
       </c>
     </row>
     <row r="13" spans="1:3">
-      <c r="A13" s="1" t="s">
-        <v>14</v>
+      <c r="A13" s="9" t="s">
+        <v>15</v>
       </c>
       <c r="B13" t="s">
         <v>5</v>
@@ -625,8 +1300,8 @@
       </c>
     </row>
     <row r="14" spans="1:3">
-      <c r="A14" s="1" t="s">
-        <v>15</v>
+      <c r="A14" s="9" t="s">
+        <v>16</v>
       </c>
       <c r="B14" t="s">
         <v>5</v>
@@ -636,8 +1311,8 @@
       </c>
     </row>
     <row r="15" spans="1:3">
-      <c r="A15" s="1" t="s">
-        <v>16</v>
+      <c r="A15" s="9" t="s">
+        <v>17</v>
       </c>
       <c r="B15" t="s">
         <v>5</v>
@@ -647,80 +1322,269 @@
       </c>
     </row>
     <row r="16" spans="1:3">
-      <c r="A16" s="1" t="s">
-        <v>17</v>
+      <c r="A16" s="9" t="s">
+        <v>18</v>
       </c>
       <c r="B16" t="s">
+        <v>5</v>
+      </c>
+      <c r="C16" s="10">
+        <v>42927</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2">
+      <c r="A17" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="B17" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3">
+      <c r="A18" s="9" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="17" spans="1:3">
-      <c r="A17" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B17" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3">
-      <c r="A18" s="1" t="s">
+      <c r="B18" t="s">
+        <v>5</v>
+      </c>
+      <c r="C18" s="8">
+        <v>42893</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3">
+      <c r="A19" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="B19" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="C19" s="8">
+        <v>42893</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3">
+      <c r="A20" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="B20" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="B18" t="s">
-        <v>5</v>
-      </c>
-      <c r="C18" s="7">
-        <v>42893</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3">
-      <c r="A19" s="5" t="s">
+      <c r="C20" s="7"/>
+    </row>
+    <row r="21" spans="1:2">
+      <c r="A21" t="s">
+        <v>24</v>
+      </c>
+      <c r="B21" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2">
+      <c r="A22" t="s">
         <v>25</v>
       </c>
-      <c r="B19" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="C19" s="7">
-        <v>42893</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3">
-      <c r="A20" s="5" t="s">
+      <c r="B22" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2">
+      <c r="A23" t="s">
         <v>26</v>
       </c>
-      <c r="B20" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="C20" s="6"/>
+      <c r="B23" t="s">
+        <v>20</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:C1"/>
   </mergeCells>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B1:B1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B$1:B$1048576">
       <formula1>"Pending, In Progress, Done, Blocked, On Hold"</formula1>
     </dataValidation>
   </dataValidations>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="1" orientation="portrait"/>
+  <headerFooter/>
   <tableParts count="1">
-    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId1"/>
   </tableParts>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr/>
+  <dimension ref="A1:E7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="6" outlineLevelCol="4"/>
+  <cols>
+    <col min="1" max="2" width="14.1428571428571" customWidth="1"/>
+    <col min="3" max="3" width="29.4285714285714" customWidth="1"/>
+    <col min="5" max="5" width="11.4285714285714" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="A1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C2" t="s">
+        <v>34</v>
+      </c>
+      <c r="D2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E2" s="2">
+        <v>42933</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" t="s">
+        <v>32</v>
+      </c>
+      <c r="B3" t="s">
+        <v>33</v>
+      </c>
+      <c r="C3" t="s">
+        <v>35</v>
+      </c>
+      <c r="D3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E3" s="2">
+        <v>42933</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" t="s">
+        <v>32</v>
+      </c>
+      <c r="B4" t="s">
+        <v>33</v>
+      </c>
+      <c r="C4" t="s">
+        <v>36</v>
+      </c>
+      <c r="D4" t="s">
+        <v>5</v>
+      </c>
+      <c r="E4" s="2">
+        <v>42933</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" t="s">
+        <v>32</v>
+      </c>
+      <c r="B5" t="s">
+        <v>33</v>
+      </c>
+      <c r="C5" t="s">
+        <v>37</v>
+      </c>
+      <c r="D5" t="s">
+        <v>5</v>
+      </c>
+      <c r="E5" s="2">
+        <v>42933</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" t="s">
+        <v>32</v>
+      </c>
+      <c r="B6" t="s">
+        <v>38</v>
+      </c>
+      <c r="C6" t="s">
+        <v>39</v>
+      </c>
+      <c r="D6" t="s">
+        <v>5</v>
+      </c>
+      <c r="E6" s="2">
+        <v>42933</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7" t="s">
+        <v>40</v>
+      </c>
+      <c r="B7" t="s">
+        <v>41</v>
+      </c>
+      <c r="C7" t="s">
+        <v>42</v>
+      </c>
+      <c r="D7" t="s">
+        <v>5</v>
+      </c>
+      <c r="E7" s="2">
+        <v>42933</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
+  <headerFooter/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr/>
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15"/>
+  <sheetData/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr/>
   <dimension ref="A1:A6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2:A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="5"/>
   <cols>
-    <col min="1" max="1" width="11.42578125" customWidth="1"/>
+    <col min="1" max="1" width="11.4285714285714" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1">
@@ -730,12 +1594,12 @@
     </row>
     <row r="2" spans="1:1">
       <c r="A2" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" t="s">
-        <v>21</v>
+        <v>43</v>
       </c>
     </row>
     <row r="4" spans="1:1">
@@ -745,16 +1609,17 @@
     </row>
     <row r="5" spans="1:1">
       <c r="A5" t="s">
-        <v>22</v>
+        <v>44</v>
       </c>
     </row>
     <row r="6" spans="1:1">
       <c r="A6" t="s">
-        <v>23</v>
+        <v>45</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555596" footer="0.51180555555555596"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
+  <headerFooter/>
   <tableParts count="1">
     <tablePart r:id="rId1"/>
   </tableParts>

</xml_diff>